<commit_message>
[Project 3] prepare submit
</commit_message>
<xml_diff>
--- a/UIUC_PSL/Project3/perf_summary.xlsx
+++ b/UIUC_PSL/Project3/perf_summary.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanyang/Dropbox/uiuc/cs598/UIUC_SPL/UIUC_PSL/Project3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yafa/Dropbox/Library/UIUC_PSL/UIUC_PSL/Project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D015ADF-9349-7741-BB9F-04C0EF2FDB01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718127EC-5A08-4A4D-A03F-4505FC74A474}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16460" activeTab="1" xr2:uid="{3E012627-85B2-4A44-A3A8-5639159FFB78}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="28040" windowHeight="16460" activeTab="1" xr2:uid="{3E012627-85B2-4A44-A3A8-5639159FFB78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>data</t>
   </si>
@@ -63,16 +62,68 @@
   </si>
   <si>
     <t>866 words selected by both Lasso and T-test</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>contribution</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>tears</t>
+  </si>
+  <si>
+    <t>masterpiece</t>
+  </si>
+  <si>
+    <t>innocence</t>
+  </si>
+  <si>
+    <t>themes</t>
+  </si>
+  <si>
+    <t>makes</t>
+  </si>
+  <si>
+    <t>beauty</t>
+  </si>
+  <si>
+    <t>highly</t>
+  </si>
+  <si>
+    <t>enjoy</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>truly</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t>film</t>
+  </si>
+  <si>
+    <t>story</t>
+  </si>
+  <si>
+    <t>made</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +133,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -254,24 +312,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -283,23 +357,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -996,66 +1063,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5D9BBC-5BEE-0D42-BB87-F74B187D8CA9}">
-  <dimension ref="B4:K12"/>
+  <dimension ref="B4:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B16" sqref="B16:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:11" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1063,31 +1130,31 @@
       <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.95858699999999997</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.94427399999999995</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>55.463982000000001</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>0.96571399999999996</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>0.94702600000000003</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>78.785514000000006</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="4">
         <v>0.96313300000000002</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>0.94484999999999997</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="5">
         <v>57.669215999999999</v>
       </c>
     </row>
@@ -1095,31 +1162,31 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.95533699999999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.94666700000000004</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>51.532507000000003</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>0.96332300000000004</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>0.94969599999999998</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>73.630443</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="4">
         <v>0.959063</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>0.94863799999999998</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="5">
         <v>53.006749999999997</v>
       </c>
     </row>
@@ -1127,31 +1194,31 @@
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>0.95606800000000003</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.946496</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>50.832053000000002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0.96298399999999995</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>0.94942000000000004</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>72.296963000000005</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="4">
         <v>0.95842000000000005</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>0.94903199999999999</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="5">
         <v>51.825682999999998</v>
       </c>
     </row>
@@ -1159,31 +1226,31 @@
       <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.95597399999999999</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.94671400000000006</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>49.276339</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>0.96207100000000001</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>0.949183</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>82.018563</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="4">
         <v>0.95877100000000004</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>0.948322</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="5">
         <v>47.224415</v>
       </c>
     </row>
@@ -1191,35 +1258,166 @@
       <c r="B11" s="1">
         <v>4</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>0.95628000000000002</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.94661300000000004</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>50.102755000000002</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>0.96361300000000005</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>0.94886000000000004</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>80.010679999999994</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="6">
         <v>0.959619</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="7">
         <v>0.94824399999999998</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="8">
         <v>50.985306000000001</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="14"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.65901024454201296</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.464674790834045</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0.38625577955699902</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="16">
+        <v>0.37838579668583999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0.34497046296608302</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0.29170352791486598</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0.239111311716276</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0.20765276989099901</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0.198006027923218</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="16">
+        <v>0.16843686110262401</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="16">
+        <v>0.13207275853949099</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="16">
+        <v>7.0675555324880804E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="16">
+        <v>4.3030564595830899E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="16">
+        <v>-6.5045691066408099E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="16">
+        <v>-7.0519456376865797E-2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C5:E5"/>
@@ -1227,5 +1425,6 @@
     <mergeCell ref="I5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>